<commit_message>
docs are saved to BD
</commit_message>
<xml_diff>
--- a/documents/targets/targ1.xlsx
+++ b/documents/targets/targ1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t>Номер</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Пласт</t>
   </si>
   <si>
-    <t>Акутальность</t>
-  </si>
-  <si>
     <t>Т1</t>
   </si>
   <si>
@@ -55,6 +52,12 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>Актуальность</t>
+  </si>
+  <si>
+    <t>Юг1</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -416,7 +419,7 @@
         <v>1357</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -430,8 +433,11 @@
       <c r="F2">
         <v>20</v>
       </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -439,7 +445,7 @@
         <v>1357</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -453,8 +459,11 @@
       <c r="F3">
         <v>10</v>
       </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -462,7 +471,7 @@
         <v>1357</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -476,8 +485,11 @@
       <c r="F4">
         <v>5</v>
       </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -485,7 +497,7 @@
         <v>1358</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -499,8 +511,11 @@
       <c r="F5">
         <v>20</v>
       </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -508,7 +523,7 @@
         <v>1358</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -522,8 +537,11 @@
       <c r="F6">
         <v>10</v>
       </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -531,7 +549,7 @@
         <v>1358</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -545,8 +563,11 @@
       <c r="F7">
         <v>5</v>
       </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -554,7 +575,7 @@
         <v>1359</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -568,8 +589,11 @@
       <c r="F8">
         <v>20</v>
       </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -577,7 +601,7 @@
         <v>1359</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -591,8 +615,11 @@
       <c r="F9">
         <v>10</v>
       </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -600,7 +627,7 @@
         <v>1359</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -614,8 +641,11 @@
       <c r="F10">
         <v>5</v>
       </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>